<commit_message>
Completed implementation of observation_period, visit_occurrence, procedure_occurrence tables in MAINtransform. Added input to MAINextraction to select max number of samples to save.
</commit_message>
<xml_diff>
--- a/02-Transform/VocabulariesConceptMap/vocabulary.xlsx
+++ b/02-Transform/VocabulariesConceptMap/vocabulary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t xml:space="preserve">TableName</t>
   </si>
@@ -74,6 +74,54 @@
   </si>
   <si>
     <t xml:space="preserve">This is the standard marker for “Unknown” in the Race domain, as stated in the official v5.4 specs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">observation_period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">period_type_concept_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EHR encounter record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visit_occurrence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visit_type_concept_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visit_concept_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laboratory Visit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">procedure_occurrence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">procedure_type_concept_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">procedure_concept_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AmbulatoryECG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambulatory ECG (this is used for short, less-than-12-lead ECG recordings)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12LeadECG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Lead ECG (this is used for short 12-lead ECG recordings)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HolterECG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Hour ECG (this is used for longer ECG recordings, either 12-lead or not)</t>
   </si>
 </sst>
 </file>
@@ -289,15 +337,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="54.68"/>
@@ -407,6 +456,125 @@
       </c>
       <c r="E6" s="2" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>32827</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>32827</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>32036</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>32827</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>4065278</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>4145308</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>4098508</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved mapToConceptsFromVocab enabling non-exact matches (strcmpi) of SourceTerms in vocabularies. Completed condition_occurrence implementation in MAINtransform.
</commit_message>
<xml_diff>
--- a/02-Transform/VocabulariesConceptMap/vocabulary.xlsx
+++ b/02-Transform/VocabulariesConceptMap/vocabulary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="99">
   <si>
     <t xml:space="preserve">TableName</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Description (free text field for notes)</t>
   </si>
   <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
     <t xml:space="preserve">person</t>
   </si>
   <si>
@@ -122,6 +125,198 @@
   </si>
   <si>
     <t xml:space="preserve">24 Hour ECG (this is used for longer ECG recordings, either 12-lead or not)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">condition_occurrence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">condition_type_concept_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ManuallyReported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EHR problem list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StandardAnnotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AutomaticallyDetected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">condition_concept_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acute MI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acute myocardial infarction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manually reported diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coronary artery disease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obliterative coronary artery disease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earlier MI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myocardial infarction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinus node dysfunction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transient ischemic attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transient ischemic attack due to embolism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arterial hypertension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypertensive disorder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left ventricular hypertrophy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bundle branch block beat (unspecified)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bundle branch block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECG Physionet standard annotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right bundle branch block beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right bundle branch block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left bundle branch block beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left bundle branch block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supraventricular premature or ectopic beat (atrial or nodal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supraventricular premature beats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atrial escape beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atrial escape complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premature ventricular contraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventricular premature complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-on-T premature ventricular contraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fusion of ventricular and normal beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fusion beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fusion of paced and normal beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atrial premature beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atrial premature complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aberrated atrial premature beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nodal (junctional) escape beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junctional escape beats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nodal (junctional) premature beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junctional premature beats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paced beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhythm from artificial pacing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supraventricular escape beat (atrial or nodal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventricular escape beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1dAVb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First degree atrioventricular block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatically detected (Ribeiro)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atrial fibrillation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBBB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RBBB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinus bradycardia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinus tachycardia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit_concept_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent (unit of measurement)</t>
   </si>
 </sst>
 </file>
@@ -337,20 +532,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="54.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,212 +564,863 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>8532</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>8507</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>4214687</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1546846</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>32827</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>32827</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>32036</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>32827</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>4065278</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>4145308</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>4098508</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>32840</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>32827</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>32880</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>312327</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>4168972</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>4329847</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>317302</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>46272244</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>316866</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>4184746</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>313791</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>314059</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>316998</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>441872</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>4088986</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>4089462</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>4089462</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>4092012</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>4092012</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>4115173</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>4115173</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>4166380</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>4218739</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>4304202</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>4327066</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>4327066</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>314379</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>313217</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>316998</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>314059</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>4171683</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>4007310</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>8554</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added transform and load phase to example. MAINtransform completed (added observation table) and tested; table assembling still to be separated. Added MAINload, completed and tested.
</commit_message>
<xml_diff>
--- a/02-Transform/VocabulariesConceptMap/vocabulary.xlsx
+++ b/02-Transform/VocabulariesConceptMap/vocabulary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="155">
   <si>
     <t xml:space="preserve">TableName</t>
   </si>
@@ -382,7 +382,7 @@
     <t xml:space="preserve">RMSSD</t>
   </si>
   <si>
-    <t xml:space="preserve">Root Mean Squared of Successive Differences (RMSSD)</t>
+    <t xml:space="preserve">Root Mean Squared Successive Differences (RMSSD)</t>
   </si>
   <si>
     <t xml:space="preserve">HF_POWER_FFT</t>
@@ -412,7 +412,7 @@
     <t xml:space="preserve">LF_TO_HF_FFT</t>
   </si>
   <si>
-    <t xml:space="preserve">Ratio of HRV Low Frequency and High Frequency powers</t>
+    <t xml:space="preserve">Ratio of HRV Low and High Frequency powers</t>
   </si>
   <si>
     <t xml:space="preserve">VLF_POWER_FFT</t>
@@ -460,6 +460,12 @@
     <t xml:space="preserve">observation</t>
   </si>
   <si>
+    <t xml:space="preserve">observation_type_concept_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obs_event_field_concept_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">observation_source_concept_id</t>
   </si>
   <si>
@@ -469,13 +475,13 @@
     <t xml:space="preserve">Digital Sampling Rate (non-standard concept to associate with “Sampling – action”)</t>
   </si>
   <si>
-    <t xml:space="preserve">observation_concept_it</t>
+    <t xml:space="preserve">observation_concept_id</t>
   </si>
   <si>
     <t xml:space="preserve">Sampling – action</t>
   </si>
   <si>
-    <t xml:space="preserve">hertz</t>
+    <t xml:space="preserve">Hz</t>
   </si>
   <si>
     <t xml:space="preserve">Hertz (unit of measurement)</t>
@@ -704,10 +710,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E62" activeCellId="0" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1969,7 +1975,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>145</v>
       </c>
@@ -1977,13 +1983,13 @@
         <v>146</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>147</v>
+        <v>21</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>37533243</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>148</v>
+        <v>32827</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,33 +1997,67 @@
         <v>145</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>147</v>
+        <v>28</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>4117495</v>
+        <v>1147301</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>145</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D71" s="1" t="n">
+        <v>37533243</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D72" s="1" t="n">
+        <v>4117495</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D71" s="1" t="n">
+      <c r="C73" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D73" s="1" t="n">
         <v>9521</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>152</v>
+      <c r="E73" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved script and function help/comments (completed translation from Ita to Eng), repo organization, small fixes
</commit_message>
<xml_diff>
--- a/02-Transform/VocabulariesConceptMap/vocabulary.xlsx
+++ b/02-Transform/VocabulariesConceptMap/vocabulary.xlsx
@@ -712,8 +712,8 @@
   </sheetPr>
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E62" activeCellId="0" sqref="E62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E61" activeCellId="0" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
README updated with instructions on how to set up the OMOP CDM DB. Small fixes
</commit_message>
<xml_diff>
--- a/02-Transform/VocabulariesConceptMap/vocabulary.xlsx
+++ b/02-Transform/VocabulariesConceptMap/vocabulary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="154">
   <si>
     <t xml:space="preserve">TableName</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">FEMALE (standard concept for gender)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vocabularies (you can have multiple of them in the same folder or a single one for all tables; your choice) to be used with the ecg2omop pipeline comprises: 1) a TableName column, with the exact name of the OMOP table the mapped concept refers to; 2) a FieldName column, with the name of the field in which that concept can be inserted (if the same concept is allowed in multiple TableName-FieldName pairs, it must be specified each time; 3) a SourceTerm column, specifying the “standardized” term (i.e., a string, which will be searched with EXACT MATCH to ensure integrity and minimize risks of mistakes; so be accurate!) chosen in our Extraction routine to refer to a specific concept, attribute categorical value, variable name, etc.; 4) an OMOPconceptID column, indicating the concept ID in the OMOP CDM vocabularies to which the specified source term will be mapped; 5) a Description column where free text notes and considerations can be reported; in particular, we should always include the textual description of the selected OMOP concept; this column (and possibly following ones) will never be imported in Matlab, so feel free to use this textual field as you wish.</t>
   </si>
   <si>
     <t xml:space="preserve">M</t>
@@ -566,7 +563,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -581,10 +578,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -712,8 +705,8 @@
   </sheetPr>
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E61" activeCellId="0" sqref="E61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -762,9 +755,7 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -774,13 +765,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>8507</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,13 +782,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>4214687</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -805,16 +796,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1546846</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,1242 +813,1242 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>32827</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>32827</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>32036</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>32827</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>4065278</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>4145308</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>4098508</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>32840</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>32827</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>32880</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>312327</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>4168972</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>4329847</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>317302</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>46272244</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>316866</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>4184746</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>313791</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>314059</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>316998</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>441872</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>4088986</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>4089462</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>4089462</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>4092012</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>4092012</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33" s="1" t="n">
         <v>4115173</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>4115173</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D35" s="1" t="n">
         <v>4166380</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D36" s="1" t="n">
         <v>4218739</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>4304202</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>4327066</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D39" s="1" t="n">
         <v>4327066</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>314379</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>313217</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="1" t="n">
         <v>316998</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D43" s="1" t="n">
         <v>314059</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D44" s="1" t="n">
         <v>4171683</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D45" s="1" t="n">
         <v>4007310</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="C46" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D46" s="1" t="n">
         <v>32827</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D47" s="1" t="n">
         <v>1147301</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="D48" s="1" t="n">
         <v>8554</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>8555</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="D49" s="4" t="n">
-        <v>8555</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>9593</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D50" s="4" t="n">
-        <v>9593</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>8523</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D51" s="4" t="n">
-        <v>8523</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>9260</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D52" s="4" t="n">
-        <v>9260</v>
-      </c>
-      <c r="E52" s="1" t="s">
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="D53" s="1" t="n">
+        <v>3004182</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D53" s="0" t="n">
-        <v>3004182</v>
-      </c>
-      <c r="E53" s="0" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C54" s="0" t="s">
+      <c r="D54" s="1" t="n">
+        <v>3006307</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D54" s="0" t="n">
-        <v>3006307</v>
-      </c>
-      <c r="E54" s="0" t="s">
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="0" t="s">
+      <c r="D55" s="1" t="n">
+        <v>21491502</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="0" t="n">
-        <v>21491502</v>
-      </c>
-      <c r="E55" s="0" t="s">
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="D56" s="1" t="n">
         <v>2000000001</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>121</v>
       </c>
       <c r="D57" s="1" t="n">
         <v>2000000002</v>
       </c>
-      <c r="E57" s="0" t="s">
+      <c r="E57" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>123</v>
       </c>
       <c r="D58" s="1" t="n">
         <v>2000000003</v>
       </c>
-      <c r="E58" s="0" t="s">
+      <c r="E58" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B59" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="D59" s="1" t="n">
         <v>2000000004</v>
       </c>
-      <c r="E59" s="0" t="s">
+      <c r="E59" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="D60" s="1" t="n">
         <v>2000000005</v>
       </c>
-      <c r="E60" s="0" t="s">
+      <c r="E60" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="D61" s="1" t="n">
         <v>2000000006</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>131</v>
       </c>
       <c r="D62" s="1" t="n">
         <v>2000000007</v>
       </c>
-      <c r="E62" s="0" t="s">
+      <c r="E62" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="D63" s="1" t="n">
         <v>2000000008</v>
       </c>
-      <c r="E63" s="0" t="s">
+      <c r="E63" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B64" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="D64" s="1" t="n">
         <v>2000000009</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="D65" s="1" t="n">
         <v>2000000010</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="D66" s="1" t="n">
         <v>2000000011</v>
       </c>
       <c r="E66" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="D67" s="1" t="n">
         <v>2000000012</v>
       </c>
       <c r="E67" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="D68" s="1" t="n">
         <v>2000000013</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="C69" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D69" s="1" t="n">
         <v>32827</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D70" s="1" t="n">
         <v>1147301</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>37533243</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D72" s="1" t="n">
         <v>4117495</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D73" s="1" t="n">
         <v>9521</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>